<commit_message>
add sownload excel for all
</commit_message>
<xml_diff>
--- a/assets/Excel- template.xlsx
+++ b/assets/Excel- template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xampp\htdocs\piat_checklist\piat_checklist\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xampp\htdocs\piat\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1146,6 +1146,36 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1170,35 +1200,23 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1244,24 +1262,6 @@
     </xf>
     <xf numFmtId="15" fontId="9" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1588,7 +1588,7 @@
   <dimension ref="B1:AP37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1671,114 +1671,114 @@
       <c r="AN4" s="48"/>
     </row>
     <row r="6" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="95" t="s">
+      <c r="B6" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="87" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="87" t="s">
         <v>158</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="87" t="s">
         <v>157</v>
       </c>
-      <c r="I6" s="95" t="s">
+      <c r="I6" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="J6" s="94" t="s">
+      <c r="J6" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="99" t="s">
+      <c r="K6" s="91" t="s">
         <v>154</v>
       </c>
       <c r="L6" s="81"/>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="88" t="s">
         <v>152</v>
       </c>
-      <c r="N6" s="97" t="s">
+      <c r="N6" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="O6" s="98"/>
-      <c r="P6" s="91" t="s">
+      <c r="O6" s="90"/>
+      <c r="P6" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="93"/>
-      <c r="S6" s="91" t="s">
+      <c r="Q6" s="84"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="93"/>
-      <c r="W6" s="85" t="s">
+      <c r="T6" s="84"/>
+      <c r="U6" s="84"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="X6" s="88" t="s">
+      <c r="X6" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="Y6" s="88"/>
-      <c r="Z6" s="88"/>
-      <c r="AA6" s="88"/>
-      <c r="AB6" s="88" t="s">
+      <c r="Y6" s="98"/>
+      <c r="Z6" s="98"/>
+      <c r="AA6" s="98"/>
+      <c r="AB6" s="98" t="s">
         <v>147</v>
       </c>
-      <c r="AC6" s="88"/>
-      <c r="AD6" s="88"/>
-      <c r="AE6" s="88" t="s">
+      <c r="AC6" s="98"/>
+      <c r="AD6" s="98"/>
+      <c r="AE6" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="AF6" s="88"/>
-      <c r="AG6" s="88"/>
-      <c r="AH6" s="83" t="s">
+      <c r="AF6" s="98"/>
+      <c r="AG6" s="98"/>
+      <c r="AH6" s="93" t="s">
         <v>149</v>
       </c>
-      <c r="AI6" s="89" t="s">
+      <c r="AI6" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="AJ6" s="87" t="s">
+      <c r="AJ6" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="AK6" s="87" t="s">
+      <c r="AK6" s="97" t="s">
         <v>153</v>
       </c>
-      <c r="AL6" s="87" t="s">
+      <c r="AL6" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="AM6" s="85" t="s">
+      <c r="AM6" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="AN6" s="83" t="s">
+      <c r="AN6" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="AO6" s="84" t="s">
+      <c r="AO6" s="94" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:42" s="8" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="94"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="100"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="92"/>
       <c r="L7" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="M7" s="96"/>
+      <c r="M7" s="88"/>
       <c r="N7" s="75" t="s">
         <v>141</v>
       </c>
@@ -1806,7 +1806,7 @@
       <c r="V7" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="W7" s="86"/>
+      <c r="W7" s="96"/>
       <c r="X7" s="76" t="s">
         <v>118</v>
       </c>
@@ -1837,19 +1837,16 @@
       <c r="AG7" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AH7" s="83"/>
-      <c r="AI7" s="90"/>
-      <c r="AJ7" s="87"/>
-      <c r="AK7" s="87"/>
-      <c r="AL7" s="87"/>
-      <c r="AM7" s="86"/>
-      <c r="AN7" s="83"/>
-      <c r="AO7" s="84"/>
+      <c r="AH7" s="93"/>
+      <c r="AI7" s="100"/>
+      <c r="AJ7" s="97"/>
+      <c r="AK7" s="97"/>
+      <c r="AL7" s="97"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="93"/>
+      <c r="AO7" s="94"/>
     </row>
     <row r="8" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="82"/>
@@ -1892,9 +1889,7 @@
       <c r="AP8" s="69"/>
     </row>
     <row r="9" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B9" s="9">
-        <v>2</v>
-      </c>
+      <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="82"/>
@@ -1936,9 +1931,7 @@
       <c r="AO9" s="11"/>
     </row>
     <row r="10" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
-        <v>3</v>
-      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="82"/>
@@ -1980,9 +1973,7 @@
       <c r="AO10" s="11"/>
     </row>
     <row r="11" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B11" s="9">
-        <v>4</v>
-      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="82"/>
@@ -2024,9 +2015,7 @@
       <c r="AO11" s="11"/>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
-        <v>5</v>
-      </c>
+      <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="82"/>
@@ -2070,9 +2059,7 @@
       <c r="AO12" s="11"/>
     </row>
     <row r="13" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
-        <v>6</v>
-      </c>
+      <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="82"/>
@@ -2116,9 +2103,7 @@
       <c r="AO13" s="11"/>
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B14" s="9">
-        <v>7</v>
-      </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="82"/>
@@ -2160,9 +2145,7 @@
       <c r="AO14" s="11"/>
     </row>
     <row r="15" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B15" s="9">
-        <v>8</v>
-      </c>
+      <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="82"/>
@@ -2204,9 +2187,7 @@
       <c r="AO15" s="11"/>
     </row>
     <row r="16" spans="2:42" x14ac:dyDescent="0.2">
-      <c r="B16" s="9">
-        <v>9</v>
-      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="82"/>
@@ -2248,9 +2229,7 @@
       <c r="AO16" s="11"/>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="9">
-        <v>10</v>
-      </c>
+      <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="82"/>
@@ -2292,9 +2271,7 @@
       <c r="AO17" s="11"/>
     </row>
     <row r="18" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B18" s="9">
-        <v>11</v>
-      </c>
+      <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="82"/>
@@ -2336,9 +2313,7 @@
       <c r="AO18" s="11"/>
     </row>
     <row r="19" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B19" s="9">
-        <v>12</v>
-      </c>
+      <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="82"/>
@@ -2380,9 +2355,7 @@
       <c r="AO19" s="11"/>
     </row>
     <row r="20" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B20" s="9">
-        <v>13</v>
-      </c>
+      <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="82"/>
@@ -2424,9 +2397,7 @@
       <c r="AO20" s="11"/>
     </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B21" s="9">
-        <v>14</v>
-      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="82"/>
@@ -2468,9 +2439,7 @@
       <c r="AO21" s="11"/>
     </row>
     <row r="22" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B22" s="9">
-        <v>15</v>
-      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="82"/>
@@ -2514,9 +2483,7 @@
       <c r="AO22" s="11"/>
     </row>
     <row r="23" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B23" s="9">
-        <v>16</v>
-      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="82"/>
@@ -2560,9 +2527,7 @@
       <c r="AO23" s="11"/>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="9">
-        <v>17</v>
-      </c>
+      <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="82"/>
@@ -2606,9 +2571,7 @@
       <c r="AO24" s="11"/>
     </row>
     <row r="25" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B25" s="9">
-        <v>18</v>
-      </c>
+      <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="82"/>
@@ -2652,9 +2615,7 @@
       <c r="AO25" s="11"/>
     </row>
     <row r="26" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B26" s="9">
-        <v>19</v>
-      </c>
+      <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="82"/>
@@ -2698,9 +2659,7 @@
       <c r="AO26" s="11"/>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B27" s="9">
-        <v>20</v>
-      </c>
+      <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="82"/>
@@ -2744,9 +2703,7 @@
       <c r="AO27" s="11"/>
     </row>
     <row r="28" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B28" s="9">
-        <v>21</v>
-      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="82"/>
@@ -2790,9 +2747,7 @@
       <c r="AO28" s="11"/>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="9">
-        <v>22</v>
-      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="82"/>
@@ -2836,9 +2791,7 @@
       <c r="AO29" s="11"/>
     </row>
     <row r="30" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B30" s="9">
-        <v>23</v>
-      </c>
+      <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="82"/>
@@ -2882,9 +2835,7 @@
       <c r="AO30" s="11"/>
     </row>
     <row r="31" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B31" s="9">
-        <v>24</v>
-      </c>
+      <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="82"/>
@@ -2928,9 +2879,7 @@
       <c r="AO31" s="11"/>
     </row>
     <row r="32" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B32" s="9">
-        <v>25</v>
-      </c>
+      <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="82"/>
@@ -2974,9 +2923,7 @@
       <c r="AO32" s="11"/>
     </row>
     <row r="33" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B33" s="9">
-        <v>26</v>
-      </c>
+      <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="82"/>
@@ -3020,9 +2967,7 @@
       <c r="AO33" s="11"/>
     </row>
     <row r="34" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B34" s="9">
-        <v>27</v>
-      </c>
+      <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="82"/>
@@ -3066,9 +3011,7 @@
       <c r="AO34" s="11"/>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="9">
-        <v>28</v>
-      </c>
+      <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="82"/>
@@ -3112,9 +3055,7 @@
       <c r="AO35" s="11"/>
     </row>
     <row r="36" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B36" s="9">
-        <v>29</v>
-      </c>
+      <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="82"/>
@@ -3158,9 +3099,7 @@
       <c r="AO36" s="11"/>
     </row>
     <row r="37" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B37" s="9">
-        <v>30</v>
-      </c>
+      <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="82"/>
@@ -3205,6 +3144,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AN6:AN7"/>
+    <mergeCell ref="AO6:AO7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="AH6:AH7"/>
+    <mergeCell ref="AJ6:AJ7"/>
+    <mergeCell ref="AL6:AL7"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AG6"/>
+    <mergeCell ref="AI6:AI7"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AK6:AK7"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="F6:F7"/>
@@ -3219,18 +3170,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="AN6:AN7"/>
-    <mergeCell ref="AO6:AO7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="AJ6:AJ7"/>
-    <mergeCell ref="AL6:AL7"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AG6"/>
-    <mergeCell ref="AI6:AI7"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AK6:AK7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI12:AI37">
@@ -3380,101 +3319,101 @@
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:31" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y4" s="101" t="s">
+      <c r="Y4" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="101" t="s">
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="103" t="s">
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="AD4" s="103"/>
+      <c r="AD4" s="109"/>
     </row>
     <row r="5" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="104" t="s">
+      <c r="A5" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="106" t="s">
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="G5" s="113" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="108"/>
-      <c r="I5" s="109" t="s">
+      <c r="H5" s="114"/>
+      <c r="I5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="109" t="s">
+      <c r="J5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="111" t="s">
+      <c r="K5" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="112"/>
-      <c r="M5" s="113"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="118"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="116" t="s">
+      <c r="O5" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="116" t="s">
+      <c r="P5" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="116" t="s">
+      <c r="Q5" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="85" t="s">
+      <c r="R5" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="S5" s="116" t="s">
+      <c r="S5" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="116" t="s">
+      <c r="T5" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="116" t="s">
+      <c r="U5" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="V5" s="116" t="s">
+      <c r="V5" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="85" t="s">
+      <c r="W5" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="116" t="s">
+      <c r="X5" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="117" t="s">
+      <c r="Y5" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="117" t="s">
+      <c r="Z5" s="102"/>
+      <c r="AA5" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="AB5" s="118"/>
-      <c r="AC5" s="119" t="s">
+      <c r="AB5" s="102"/>
+      <c r="AC5" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="AD5" s="120"/>
-      <c r="AE5" s="121" t="s">
+      <c r="AD5" s="104"/>
+      <c r="AE5" s="105" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:31" s="8" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="94"/>
-      <c r="B6" s="104"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="30" t="s">
         <v>32</v>
       </c>
@@ -3484,15 +3423,15 @@
       <c r="E6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="106"/>
+      <c r="F6" s="112"/>
       <c r="G6" s="43" t="s">
         <v>128</v>
       </c>
       <c r="H6" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
       <c r="K6" s="30" t="s">
         <v>32</v>
       </c>
@@ -3502,17 +3441,17 @@
       <c r="M6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="N6" s="115"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="86"/>
-      <c r="S6" s="116"/>
-      <c r="T6" s="116"/>
-      <c r="U6" s="116"/>
-      <c r="V6" s="116"/>
-      <c r="W6" s="86"/>
-      <c r="X6" s="116"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="106"/>
+      <c r="R6" s="96"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
+      <c r="V6" s="106"/>
+      <c r="W6" s="96"/>
+      <c r="X6" s="106"/>
       <c r="Y6" s="58" t="s">
         <v>12</v>
       </c>
@@ -3531,7 +3470,7 @@
       <c r="AD6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AE6" s="121"/>
+      <c r="AE6" s="105"/>
     </row>
     <row r="7" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
@@ -6633,16 +6572,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AA4:AB4"/>
@@ -6659,6 +6588,16 @@
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6713,27 +6652,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="bc2e0d49-1918-42f8-8bb4-e4131a43c460">RQFUJF73TENJ-620-105</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="bc2e0d49-1918-42f8-8bb4-e4131a43c460">
-      <Url>http://livewire.tnb.com.my/sites/DN/PSI-TNBD/keyprocess/_layouts/15/DocIdRedir.aspx?ID=RQFUJF73TENJ-620-105</Url>
-      <Description>RQFUJF73TENJ-620-105</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004C19C044B4923240BE3E57DB03D26C23" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd2dfdea401acdad20bcb9a05de34933">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc2e0d49-1918-42f8-8bb4-e4131a43c460" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ac783bff1e70b0d91d7a40fb7bcaf6e" ns2:_="">
     <xsd:import namespace="bc2e0d49-1918-42f8-8bb4-e4131a43c460"/>
@@ -6878,6 +6796,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="bc2e0d49-1918-42f8-8bb4-e4131a43c460">RQFUJF73TENJ-620-105</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="bc2e0d49-1918-42f8-8bb4-e4131a43c460">
+      <Url>http://livewire.tnb.com.my/sites/DN/PSI-TNBD/keyprocess/_layouts/15/DocIdRedir.aspx?ID=RQFUJF73TENJ-620-105</Url>
+      <Description>RQFUJF73TENJ-620-105</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F8687D7-25B6-4B53-B2A6-E0A6ED5FD86D}">
   <ds:schemaRefs>
@@ -6887,9 +6826,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{342EADFA-DB4C-400C-9109-F92729F10E58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E3EA18-778A-4B0F-901B-808E0302BEF1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bc2e0d49-1918-42f8-8bb4-e4131a43c460"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6905,19 +6854,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E3EA18-778A-4B0F-901B-808E0302BEF1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{342EADFA-DB4C-400C-9109-F92729F10E58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bc2e0d49-1918-42f8-8bb4-e4131a43c460"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>